<commit_message>
Added MyAddress test, MyPersonalInfoTests and MyWishListTests
</commit_message>
<xml_diff>
--- a/data/TestPlan.xlsx
+++ b/data/TestPlan.xlsx
@@ -4,19 +4,23 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="logout" sheetId="2" r:id="rId2"/>
+    <sheet name="addNewAddress" sheetId="4" r:id="rId3"/>
+    <sheet name="updateAddress" sheetId="3" r:id="rId4"/>
+    <sheet name="removeAddress" sheetId="5" r:id="rId5"/>
+    <sheet name="personalInfo" sheetId="6" r:id="rId6"/>
+    <sheet name="addWishList" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="125">
   <si>
     <t>Test case id:</t>
   </si>
@@ -48,15 +52,9 @@
     <t xml:space="preserve"> MyStore web app is open</t>
   </si>
   <si>
-    <t>Click on the LogIn tab</t>
-  </si>
-  <si>
     <t>Sign in page is open</t>
   </si>
   <si>
-    <t>Click on the Email address label</t>
-  </si>
-  <si>
     <t>Mouse cursor is visible I the label</t>
   </si>
   <si>
@@ -66,9 +64,6 @@
     <t>marko.miok@gmail.com</t>
   </si>
   <si>
-    <t>Click on the Password address label</t>
-  </si>
-  <si>
     <t>Type in valid password</t>
   </si>
   <si>
@@ -87,15 +82,9 @@
     <t>bratmoj123</t>
   </si>
   <si>
-    <t>valid email addres is typed in</t>
-  </si>
-  <si>
     <t>valid password is typed in</t>
   </si>
   <si>
-    <t>Click on the Sign in button</t>
-  </si>
-  <si>
     <t>User is succsessfully signed in</t>
   </si>
   <si>
@@ -109,19 +98,324 @@
   </si>
   <si>
     <t>There is 1 error</t>
+  </si>
+  <si>
+    <t>Click Logout button</t>
+  </si>
+  <si>
+    <t>User is loged out successfully</t>
+  </si>
+  <si>
+    <t>Log out succsessfully</t>
+  </si>
+  <si>
+    <t>Profile page is open</t>
+  </si>
+  <si>
+    <t>Click on the "My Address" button</t>
+  </si>
+  <si>
+    <t>Click on the "Profile name" button</t>
+  </si>
+  <si>
+    <t>Click on the "LogIn tab"</t>
+  </si>
+  <si>
+    <t>Click on the "Password" label</t>
+  </si>
+  <si>
+    <t>Click on the "Email address" label</t>
+  </si>
+  <si>
+    <t>Click on the "Sign in" button</t>
+  </si>
+  <si>
+    <t>Valid email addres is typed in</t>
+  </si>
+  <si>
+    <t>My addresses page is open</t>
+  </si>
+  <si>
+    <t>Click on the "update" button</t>
+  </si>
+  <si>
+    <t>Profile info page is open</t>
+  </si>
+  <si>
+    <t>Click on the "Save" button</t>
+  </si>
+  <si>
+    <t>User is allready loged in</t>
+  </si>
+  <si>
+    <t>Type new address in the "Address" label</t>
+  </si>
+  <si>
+    <t>New address is typed in in the label</t>
+  </si>
+  <si>
+    <t>Type new address in the "Address (Line 2)" label</t>
+  </si>
+  <si>
+    <t>New second address is typed in in the label</t>
+  </si>
+  <si>
+    <t>Type in new city name in the "City" label</t>
+  </si>
+  <si>
+    <t>New city is typed in</t>
+  </si>
+  <si>
+    <t>Kobe Bryant rd. 7</t>
+  </si>
+  <si>
+    <t>Lakers drive 4</t>
+  </si>
+  <si>
+    <t>Los Angeles</t>
+  </si>
+  <si>
+    <t>Type in new postal code</t>
+  </si>
+  <si>
+    <t>New postal code is typed in</t>
+  </si>
+  <si>
+    <t>New alias address name is typed in</t>
+  </si>
+  <si>
+    <t>New adresses info data is now saved</t>
+  </si>
+  <si>
+    <t>Los Angeles sports finance</t>
+  </si>
+  <si>
+    <t>Hajduk Veljkova 14</t>
+  </si>
+  <si>
+    <t>Kraljevica Marka 23</t>
+  </si>
+  <si>
+    <t>Novi Sad</t>
+  </si>
+  <si>
+    <t>MM traders</t>
+  </si>
+  <si>
+    <t>Original profile data:</t>
+  </si>
+  <si>
+    <t>Alaska</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>Select country from "State" dropdown menu</t>
+  </si>
+  <si>
+    <t>Type in new alias addres name in "Please assign an address title for future reference. " label</t>
+  </si>
+  <si>
+    <t>New country is now selected</t>
+  </si>
+  <si>
+    <t>New address data:</t>
+  </si>
+  <si>
+    <t>Sunny street 17</t>
+  </si>
+  <si>
+    <t>South beach 100</t>
+  </si>
+  <si>
+    <t>Miami</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>Boat rides</t>
+  </si>
+  <si>
+    <t>Click on the "Add a new address" button</t>
+  </si>
+  <si>
+    <t>055777999</t>
+  </si>
+  <si>
+    <t>0603335555</t>
+  </si>
+  <si>
+    <t>Type in a new mobile number</t>
+  </si>
+  <si>
+    <t>New mobile number is typed in</t>
+  </si>
+  <si>
+    <t>Adding second addres with valid credentials</t>
+  </si>
+  <si>
+    <t>063444789</t>
+  </si>
+  <si>
+    <t>Update address with valid credentials</t>
+  </si>
+  <si>
+    <t>Remove address succsessfully</t>
+  </si>
+  <si>
+    <t>Click on the "delete" button</t>
+  </si>
+  <si>
+    <t>Address is deleted now</t>
+  </si>
+  <si>
+    <t>"Are you sure" message pops up</t>
+  </si>
+  <si>
+    <t>Click on the confirm button on the pop up message</t>
+  </si>
+  <si>
+    <t>Update personal info page</t>
+  </si>
+  <si>
+    <t>Click on the "My personal info" button</t>
+  </si>
+  <si>
+    <t>My personal info page is open</t>
+  </si>
+  <si>
+    <t>Type in the new name in "First name" label</t>
+  </si>
+  <si>
+    <t>Type in the new last name in "Last name" label</t>
+  </si>
+  <si>
+    <t>New name is typed in now</t>
+  </si>
+  <si>
+    <t>New last name is typed in now</t>
+  </si>
+  <si>
+    <t>Type in the new email in "E-mail address" label</t>
+  </si>
+  <si>
+    <t>New email address is typed in now</t>
+  </si>
+  <si>
+    <t>Type in current password in "current password" label</t>
+  </si>
+  <si>
+    <t>Current password is typed in now</t>
+  </si>
+  <si>
+    <t>mare.care@mm.com</t>
+  </si>
+  <si>
+    <t>Katic</t>
+  </si>
+  <si>
+    <t>Rasko</t>
+  </si>
+  <si>
+    <t>Marko</t>
+  </si>
+  <si>
+    <t>Miokovic</t>
+  </si>
+  <si>
+    <t>Assert changes</t>
+  </si>
+  <si>
+    <t>Saved changes are confirmed</t>
+  </si>
+  <si>
+    <t>Your personal information has been successfully updated.</t>
+  </si>
+  <si>
+    <t>Click on the "My wish list" button</t>
+  </si>
+  <si>
+    <t>My wish list page is open</t>
+  </si>
+  <si>
+    <t>Type in wish list name in "Name" label</t>
+  </si>
+  <si>
+    <t>New wish list name is typed in</t>
+  </si>
+  <si>
+    <t>milenasWishList</t>
+  </si>
+  <si>
+    <t>New wish list is created</t>
+  </si>
+  <si>
+    <t>Assert that new wish list is created</t>
+  </si>
+  <si>
+    <t>Assert is confirmed</t>
+  </si>
+  <si>
+    <t>Adding a wish list successfully</t>
+  </si>
+  <si>
+    <t>mladensWishList</t>
+  </si>
+  <si>
+    <t>Third wish list data:</t>
+  </si>
+  <si>
+    <t>Second wish list data:</t>
+  </si>
+  <si>
+    <t>slobodansWishList</t>
+  </si>
+  <si>
+    <t>Forth wish list:</t>
+  </si>
+  <si>
+    <t>milansWishList</t>
+  </si>
+  <si>
+    <t>BOAT RIDES</t>
+  </si>
+  <si>
+    <t>LOS ANGELES SPORTS FINANCE</t>
+  </si>
+  <si>
+    <t>Assert that address is successfully updated</t>
+  </si>
+  <si>
+    <t>Address is successfully updated</t>
+  </si>
+  <si>
+    <t>Assert that address is successfully added</t>
+  </si>
+  <si>
+    <t>Address is successfully added</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -144,13 +438,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -448,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -482,13 +788,13 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="30">
@@ -515,79 +821,79 @@
     </row>
     <row r="4" spans="1:8">
       <c r="D4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="D7" s="1" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="D8" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F8" s="1">
         <v>123456789</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="D9" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="D10" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -598,24 +904,957 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="33.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="44.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="45">
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="D4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="D5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="D7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="D8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="1">
+        <v>123456789</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="D9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="D10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="D11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="44.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="44.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="45">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="D3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="D4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="D5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="D6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="D7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="D8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="D9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="3">
+        <v>23999</v>
+      </c>
+      <c r="G9" s="3">
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="D10" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="45">
+      <c r="C11" s="5"/>
+      <c r="D11" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="C12" s="5"/>
+      <c r="D12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="C13" s="5"/>
+      <c r="D13" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="F10:G10" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="44.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="44.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="29.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="45">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="D3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="D4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="D5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="D6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="D7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="D8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="D9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="3">
+        <v>77777</v>
+      </c>
+      <c r="G9" s="3">
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="D10" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="45">
+      <c r="C11" s="5"/>
+      <c r="D11" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="C12" s="5"/>
+      <c r="D12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="C13" s="5"/>
+      <c r="D13" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="F10:G10" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="46.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="44.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="D3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="D4" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="D5" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="C11" s="5"/>
+      <c r="D11" s="4"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="44.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="44.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="D3" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="D4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="D5" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="D6" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30">
+      <c r="D7" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7" s="3">
+        <v>123456789</v>
+      </c>
+      <c r="G7" s="3">
+        <v>123456789</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="D8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" spans="1:7" ht="45">
+      <c r="C9" s="5"/>
+      <c r="D9" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="F11" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J12"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="33" style="3" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="21" style="3" customWidth="1"/>
+    <col min="8" max="9" width="18.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" style="3" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="30">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="D3" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="D4" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="D5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="D6" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="C10" s="5"/>
+      <c r="D10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>